<commit_message>
Starting to get things stood up.
</commit_message>
<xml_diff>
--- a/KanBanBoard.xlsx
+++ b/KanBanBoard.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
   <si>
     <t>Task</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Project Refence</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>User Story: As the Mentor I would like my Mentee to read through the Solution Map and create the project references there in.</t>
@@ -90,13 +87,71 @@
 StructureMap
 Machine.Fakes.Rinomocks (Adding this one will add a handful of others)
 </t>
+  </si>
+  <si>
+    <t>Primary Function</t>
+  </si>
+  <si>
+    <t>User Story: As a Video Game Junky I want to be able to write and comment on reviews submitted to this site.</t>
+  </si>
+  <si>
+    <t>Secondary Function</t>
+  </si>
+  <si>
+    <t>User Story: As a Video Game Junky I want to be able to register to Game RSS Feeds of my choice and have them display on my front page.</t>
+  </si>
+  <si>
+    <t>User Story: As a VGJ I want to be able to register on the site and have an account.</t>
+  </si>
+  <si>
+    <t>User Story: As a VGJ I want to be able to Categorize Reviews by Gener, Manufacturer, and System</t>
+  </si>
+  <si>
+    <t>User Story: As a VGJ I want to be able to Vote on Reviews as a way of showing how much I liked/Hated them. Make system Gamer Friendly with Flames vs Bonus Lives.</t>
+  </si>
+  <si>
+    <t>User Story: As a VGJ I would like to be able to submit Hints/Cheats/Walkthroughs for games.</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Need to be able to Comment on Reviews.
+Add/Update functionaliy for Reviews.
+Reviews need to fit into Categories, see SF9.
+Need to be able to Vote on Reviews. See SF10</t>
+  </si>
+  <si>
+    <t>Users will need a DB of RSS Feeds to Select From to Subscribe to.
+Users will need functionality to add new RSS Feeds.
+Users will need functionality to remove feeds.
+User needs to be able to sort by Submit Date and Source.</t>
+  </si>
+  <si>
+    <t>User needs o be able to register with Email Address.
+User needs to be able to use FB/G+/Lito register.</t>
+  </si>
+  <si>
+    <t>User will need ability to add Genre.
+Add Manufatorure.
+Add System.
+Add Game Title.</t>
+  </si>
+  <si>
+    <t>Voting Systems are bad ass.</t>
+  </si>
+  <si>
+    <t>Will function like Comments, but will go through a review process before being live on the site.</t>
+  </si>
+  <si>
+    <t>P1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,8 +168,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +195,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -146,18 +226,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -440,108 +550,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
-    <col min="6" max="6" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="30.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="J3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="J4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
+      <c r="B6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>